<commit_message>
Updates to downloading files, evaluation plot data, and support functions. Removed saved files for testing unless requested.
</commit_message>
<xml_diff>
--- a/Instances.xlsx
+++ b/Instances.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cdc-my.sharepoint.com/personal/bzp3_cdc_gov/Documents/_Malaria/Projects/MagicGlasses2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{FAA29904-BAA7-F844-9D08-9E9F00116AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6799ACF2-7EE7-4604-9424-AE51E77BA7CA}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{FAA29904-BAA7-F844-9D08-9E9F00116AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{433C3A1F-D414-4D5E-94A7-23DE0BE2FC06}"/>
   <bookViews>
-    <workbookView xWindow="20052" yWindow="-108" windowWidth="20376" windowHeight="12360" xr2:uid="{8BA4FBCD-55B1-E647-B41A-02F2E5FD225B}"/>
+    <workbookView xWindow="3345" yWindow="2505" windowWidth="21600" windowHeight="11385" xr2:uid="{8BA4FBCD-55B1-E647-B41A-02F2E5FD225B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,22 +51,22 @@
     <t>IPaddress</t>
   </si>
   <si>
-    <t>https://play.dhis2.org/2.37/</t>
-  </si>
-  <si>
-    <t>https://play.dhis2.org/2.36/</t>
-  </si>
-  <si>
-    <t>DHIS2 Demo 2.37</t>
-  </si>
-  <si>
-    <t>DHIS2 Demo 2.36</t>
-  </si>
-  <si>
-    <t>https://play.dhis2.org/2.35/</t>
-  </si>
-  <si>
-    <t>DHIS2 Demo 2.35</t>
+    <t>DHIS2 Demo 2.40</t>
+  </si>
+  <si>
+    <t>https://play.dhis2.org/2.40/</t>
+  </si>
+  <si>
+    <t>DHIS2 Demo 2.39</t>
+  </si>
+  <si>
+    <t>https://play.dhis2.org/2.39/</t>
+  </si>
+  <si>
+    <t>DHIS2 Demo 2.38</t>
+  </si>
+  <si>
+    <t>https://play.dhis2.org/2.38/</t>
   </si>
 </sst>
 </file>
@@ -438,16 +438,16 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="60.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -461,12 +461,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -475,12 +475,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -489,12 +489,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -506,9 +506,9 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{B661CBDF-6F5E-EE45-8D8A-72BCAC2E54F6}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{829E8F59-B5CB-7044-8C71-A1051156DD5B}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{599D80BE-46DC-473F-A163-35A3C3A77C2D}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{040B7DB1-B7CB-4A76-A93B-F5D9145BF95C}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{0F12C359-025B-45E9-9705-68F4D3BDA36D}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{3B1EE631-E85C-4C9F-B3CD-45EC4D474670}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>